<commit_message>
Change picture + some design choices
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naumann\Dropbox (Privat)\lennardnau.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45920C1C-2C9B-4DE5-AB6B-EF749A9EF0AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE5C008-ACB4-4545-883A-5359A5B1533B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{3CBB864D-7064-4EC0-B319-6895944E5474}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>Power Law Distributions in Intrastate Conflict Intensity Dynamics</t>
   </si>
   <si>
-    <t>Other writing</t>
-  </si>
-  <si>
     <t>Christoph Trinn</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Conflict Management and Peace Science, 40(4)</t>
+  </si>
+  <si>
+    <t>Other work</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,261 +567,261 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
       <c r="K1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
         <v>39</v>
       </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6">
         <v>2022</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
       </c>
       <c r="F7">
         <v>2024</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
       </c>
       <c r="F8">
         <v>2022</v>
       </c>
       <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>